<commit_message>
new noise types tested
</commit_message>
<xml_diff>
--- a/SavedMetrics.xlsx
+++ b/SavedMetrics.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="12">
   <si>
     <t>Method</t>
   </si>
@@ -37,6 +37,18 @@
   </si>
   <si>
     <t>wiener</t>
+  </si>
+  <si>
+    <t>artificial_nonstat</t>
+  </si>
+  <si>
+    <t>speech_shaped</t>
+  </si>
+  <si>
+    <t>babble</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -57,7 +69,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -73,11 +85,31 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -87,6 +119,26 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -96,38 +148,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E15"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.34765625" customWidth="true"/>
-    <col min="2" max="2" width="8.34765625" customWidth="true"/>
+    <col min="2" max="2" width="15.16796875" customWidth="true"/>
     <col min="3" max="3" width="13.8046875" customWidth="true"/>
     <col min="4" max="4" width="12.7109375" customWidth="true"/>
     <col min="5" max="5" width="15.2578125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="27" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="27" t="s">
         <v>3</v>
       </c>
       <c r="C2">
@@ -136,15 +188,15 @@
       <c r="D2">
         <v>0.89332368959091768</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="28">
         <v>44348.878760439817</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="27" t="s">
         <v>3</v>
       </c>
       <c r="C3">
@@ -153,15 +205,15 @@
       <c r="D3">
         <v>0.87451280722593094</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="28">
         <v>44348.878986597221</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="27" t="s">
         <v>3</v>
       </c>
       <c r="C4">
@@ -170,15 +222,15 @@
       <c r="D4">
         <v>0.83553443275495143</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="28">
         <v>44348.879270787038</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="27" t="s">
         <v>3</v>
       </c>
       <c r="C5">
@@ -187,8 +239,178 @@
       <c r="D5">
         <v>0.85364590717783884</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="28">
         <v>44348.879523692129</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>1.4367909706378421</v>
+      </c>
+      <c r="D6">
+        <v>0.80143724456104604</v>
+      </c>
+      <c r="E6" s="28">
+        <v>44348.899145949072</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>5.4015461988098936</v>
+      </c>
+      <c r="D7">
+        <v>0.45057822768744638</v>
+      </c>
+      <c r="E7" s="28">
+        <v>44348.89997042824</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>7.3313076559317567</v>
+      </c>
+      <c r="D8">
+        <v>0.34953195044326651</v>
+      </c>
+      <c r="E8" s="28">
+        <v>44348.901890624998</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>1.3850067649187188</v>
+      </c>
+      <c r="D9">
+        <v>0.81956819527446345</v>
+      </c>
+      <c r="E9" s="28">
+        <v>44348.903402002317</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>5.4918035615967256</v>
+      </c>
+      <c r="D10">
+        <v>0.44306501455808478</v>
+      </c>
+      <c r="E10" s="28">
+        <v>44348.90401445602</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>7.5457154631522956</v>
+      </c>
+      <c r="D11">
+        <v>0.35945044540232923</v>
+      </c>
+      <c r="E11" s="28">
+        <v>44348.90454693287</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>2.926165091243039</v>
+      </c>
+      <c r="D12">
+        <v>0.84341442843208414</v>
+      </c>
+      <c r="E12" s="28">
+        <v>44348.906165578701</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>2.6956708104450637</v>
+      </c>
+      <c r="D13">
+        <v>0.82355597216753451</v>
+      </c>
+      <c r="E13" s="28">
+        <v>44348.906636956017</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>7.4009306697642767</v>
+      </c>
+      <c r="D14">
+        <v>0.48089722173903315</v>
+      </c>
+      <c r="E14" s="28">
+        <v>44348.907169513892</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>8.2025215654592216</v>
+      </c>
+      <c r="D15">
+        <v>0.424176850949609</v>
+      </c>
+      <c r="E15" s="28">
+        <v>44348.907604178239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed initial PSD estimate
</commit_message>
<xml_diff>
--- a/SavedMetrics.xlsx
+++ b/SavedMetrics.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="12">
   <si>
     <t>Method</t>
   </si>
@@ -69,7 +69,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="49">
+  <borders count="75">
     <border>
       <left/>
       <right/>
@@ -125,11 +125,37 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -179,6 +205,32 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="57" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="59" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="60" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="61" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="62" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="64" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="65" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="66" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="67" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="68" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="69" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="70" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="71" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="72" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="73" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="74" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -188,7 +240,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E38"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.34765625" customWidth="true"/>
@@ -199,27 +251,27 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="73" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="47" t="s">
+      <c r="A2" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="73" t="s">
         <v>3</v>
       </c>
       <c r="C2">
@@ -228,15 +280,15 @@
       <c r="D2">
         <v>0.89332368959091768</v>
       </c>
-      <c r="E2" s="48">
+      <c r="E2" s="74">
         <v>44348.878760439817</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="47" t="s">
+      <c r="A3" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="73" t="s">
         <v>3</v>
       </c>
       <c r="C3">
@@ -245,15 +297,15 @@
       <c r="D3">
         <v>0.87451280722593094</v>
       </c>
-      <c r="E3" s="48">
+      <c r="E3" s="74">
         <v>44348.878986597221</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="47" t="s">
+      <c r="A4" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="73" t="s">
         <v>3</v>
       </c>
       <c r="C4">
@@ -262,15 +314,15 @@
       <c r="D4">
         <v>0.83553443275495143</v>
       </c>
-      <c r="E4" s="48">
+      <c r="E4" s="74">
         <v>44348.879270787038</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="47" t="s">
+      <c r="A5" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="73" t="s">
         <v>3</v>
       </c>
       <c r="C5">
@@ -279,15 +331,15 @@
       <c r="D5">
         <v>0.85364590717783884</v>
       </c>
-      <c r="E5" s="48">
+      <c r="E5" s="74">
         <v>44348.879523692129</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="47" t="s">
+      <c r="A6" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="73" t="s">
         <v>8</v>
       </c>
       <c r="C6">
@@ -296,15 +348,15 @@
       <c r="D6">
         <v>0.80143724456104604</v>
       </c>
-      <c r="E6" s="48">
+      <c r="E6" s="74">
         <v>44348.899145949072</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="47" t="s">
+      <c r="A7" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="73" t="s">
         <v>9</v>
       </c>
       <c r="C7">
@@ -313,15 +365,15 @@
       <c r="D7">
         <v>0.45057822768744638</v>
       </c>
-      <c r="E7" s="48">
+      <c r="E7" s="74">
         <v>44348.89997042824</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="47" t="s">
+      <c r="A8" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="73" t="s">
         <v>10</v>
       </c>
       <c r="C8">
@@ -330,15 +382,15 @@
       <c r="D8">
         <v>0.34953195044326651</v>
       </c>
-      <c r="E8" s="48">
+      <c r="E8" s="74">
         <v>44348.901890624998</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="47" t="s">
+      <c r="A9" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="73" t="s">
         <v>8</v>
       </c>
       <c r="C9">
@@ -347,15 +399,15 @@
       <c r="D9">
         <v>0.81956819527446345</v>
       </c>
-      <c r="E9" s="48">
+      <c r="E9" s="74">
         <v>44348.903402002317</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="47" t="s">
+      <c r="A10" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="73" t="s">
         <v>9</v>
       </c>
       <c r="C10">
@@ -364,15 +416,15 @@
       <c r="D10">
         <v>0.44306501455808478</v>
       </c>
-      <c r="E10" s="48">
+      <c r="E10" s="74">
         <v>44348.90401445602</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="47" t="s">
+      <c r="A11" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="73" t="s">
         <v>10</v>
       </c>
       <c r="C11">
@@ -381,15 +433,15 @@
       <c r="D11">
         <v>0.35945044540232923</v>
       </c>
-      <c r="E11" s="48">
+      <c r="E11" s="74">
         <v>44348.90454693287</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="73" t="s">
         <v>3</v>
       </c>
       <c r="C12">
@@ -398,15 +450,15 @@
       <c r="D12">
         <v>0.84341442843208414</v>
       </c>
-      <c r="E12" s="48">
+      <c r="E12" s="74">
         <v>44348.906165578701</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="73" t="s">
         <v>8</v>
       </c>
       <c r="C13">
@@ -415,15 +467,15 @@
       <c r="D13">
         <v>0.82355597216753451</v>
       </c>
-      <c r="E13" s="48">
+      <c r="E13" s="74">
         <v>44348.906636956017</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="73" t="s">
         <v>9</v>
       </c>
       <c r="C14">
@@ -432,15 +484,15 @@
       <c r="D14">
         <v>0.48089722173903315</v>
       </c>
-      <c r="E14" s="48">
+      <c r="E14" s="74">
         <v>44348.907169513892</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="73" t="s">
         <v>10</v>
       </c>
       <c r="C15">
@@ -449,15 +501,15 @@
       <c r="D15">
         <v>0.424176850949609</v>
       </c>
-      <c r="E15" s="48">
+      <c r="E15" s="74">
         <v>44348.907604178239</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="73" t="s">
         <v>10</v>
       </c>
       <c r="C16">
@@ -466,15 +518,15 @@
       <c r="D16">
         <v>0.424176850949609</v>
       </c>
-      <c r="E16" s="48">
+      <c r="E16" s="74">
         <v>44350.668256516205</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="47" t="s">
+      <c r="A17" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="73" t="s">
         <v>10</v>
       </c>
       <c r="C17">
@@ -483,15 +535,15 @@
       <c r="D17">
         <v>0.35016115181009261</v>
       </c>
-      <c r="E17" s="48">
+      <c r="E17" s="74">
         <v>44350.680693229166</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="47" t="s">
+      <c r="A18" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="73" t="s">
         <v>10</v>
       </c>
       <c r="C18">
@@ -500,15 +552,15 @@
       <c r="D18">
         <v>0.34950520164578464</v>
       </c>
-      <c r="E18" s="48">
+      <c r="E18" s="74">
         <v>44350.689598310186</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="47" t="s">
+      <c r="A19" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="73" t="s">
         <v>10</v>
       </c>
       <c r="C19">
@@ -517,15 +569,15 @@
       <c r="D19">
         <v>0.35044736282974182</v>
       </c>
-      <c r="E19" s="48">
+      <c r="E19" s="74">
         <v>44350.694079594905</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="47" t="s">
+      <c r="A20" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="73" t="s">
         <v>10</v>
       </c>
       <c r="C20">
@@ -534,15 +586,15 @@
       <c r="D20">
         <v>0.34694508295690701</v>
       </c>
-      <c r="E20" s="48">
+      <c r="E20" s="74">
         <v>44350.694857858798</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="47" t="s">
+      <c r="A21" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="73" t="s">
         <v>10</v>
       </c>
       <c r="C21">
@@ -551,15 +603,15 @@
       <c r="D21">
         <v>0.35725556073937109</v>
       </c>
-      <c r="E21" s="48">
+      <c r="E21" s="74">
         <v>44350.695228182871</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="47" t="s">
+      <c r="A22" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="73" t="s">
         <v>10</v>
       </c>
       <c r="C22">
@@ -568,15 +620,15 @@
       <c r="D22">
         <v>0.21583838991045445</v>
       </c>
-      <c r="E22" s="48">
+      <c r="E22" s="74">
         <v>44350.714161412034</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="47" t="s">
+      <c r="A23" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="73" t="s">
         <v>10</v>
       </c>
       <c r="C23">
@@ -585,15 +637,15 @@
       <c r="D23">
         <v>0.21319852253565241</v>
       </c>
-      <c r="E23" s="48">
+      <c r="E23" s="74">
         <v>44350.714936469907</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="47" t="s">
+      <c r="A24" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="73" t="s">
         <v>8</v>
       </c>
       <c r="C24">
@@ -602,15 +654,15 @@
       <c r="D24">
         <v>0.36047804257180716</v>
       </c>
-      <c r="E24" s="48">
+      <c r="E24" s="74">
         <v>44350.722869189813</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="47" t="s">
+      <c r="A25" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="73" t="s">
         <v>8</v>
       </c>
       <c r="C25">
@@ -619,8 +671,229 @@
       <c r="D25">
         <v>0.81535826194874184</v>
       </c>
-      <c r="E25" s="48">
+      <c r="E25" s="74">
         <v>44350.724431782408</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26">
+        <v>7.6362942896867061</v>
+      </c>
+      <c r="D26">
+        <v>0.34694508295690701</v>
+      </c>
+      <c r="E26" s="74">
+        <v>44363.823397997687</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <v>7.7535234951987304</v>
+      </c>
+      <c r="D27">
+        <v>0.35725556073937109</v>
+      </c>
+      <c r="E27" s="74">
+        <v>44363.831082418983</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <v>6.9249081387883082</v>
+      </c>
+      <c r="D28">
+        <v>0.34195716776819013</v>
+      </c>
+      <c r="E28" s="74">
+        <v>44363.835290937503</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29">
+        <v>4.6373008021971254</v>
+      </c>
+      <c r="D29">
+        <v>0.46123988143192723</v>
+      </c>
+      <c r="E29" s="74">
+        <v>44363.837339571757</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30">
+        <v>4.8547821281961383</v>
+      </c>
+      <c r="D30">
+        <v>0.46743214664098398</v>
+      </c>
+      <c r="E30" s="74">
+        <v>44363.83948466435</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <v>4.8532915562916497</v>
+      </c>
+      <c r="D31">
+        <v>0.46735679086905524</v>
+      </c>
+      <c r="E31" s="74">
+        <v>44363.840346921294</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <v>5.1315481978890469</v>
+      </c>
+      <c r="D32">
+        <v>0.46789558446130164</v>
+      </c>
+      <c r="E32" s="74">
+        <v>44363.840715069447</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33">
+        <v>4.5520632440287621</v>
+      </c>
+      <c r="D33">
+        <v>0.46057844367276046</v>
+      </c>
+      <c r="E33" s="74">
+        <v>44363.863135243053</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34">
+        <v>4.7881466901084702</v>
+      </c>
+      <c r="D34">
+        <v>0.46750753451980886</v>
+      </c>
+      <c r="E34" s="74">
+        <v>44363.864021712965</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35">
+        <v>5.4154610985152773</v>
+      </c>
+      <c r="D35">
+        <v>0.45969432948021999</v>
+      </c>
+      <c r="E35" s="74">
+        <v>44363.86481684028</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36">
+        <v>4.7881466901084702</v>
+      </c>
+      <c r="D36">
+        <v>0.46750753451980886</v>
+      </c>
+      <c r="E36" s="74">
+        <v>44363.86929855324</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37">
+        <v>6.8838355664358808</v>
+      </c>
+      <c r="D37">
+        <v>0.34149152460286392</v>
+      </c>
+      <c r="E37" s="74">
+        <v>44363.87002451389</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38">
+        <v>7.2327302179446615</v>
+      </c>
+      <c r="D38">
+        <v>0.35016987918396275</v>
+      </c>
+      <c r="E38" s="74">
+        <v>44363.870556307869</v>
       </c>
     </row>
   </sheetData>

</xml_diff>